<commit_message>
Added const for yield
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -647,7 +647,11 @@
       <c r="Q5" t="n">
         <v>6</v>
       </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S5" t="n">
         <v>0.03</v>
       </c>
@@ -687,7 +691,11 @@
       <c r="Q6" t="n">
         <v>6</v>
       </c>
-      <c r="R6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S6" t="n">
         <v>0.12</v>
       </c>
@@ -727,7 +735,11 @@
       <c r="Q7" t="n">
         <v>6</v>
       </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S7" t="n">
         <v>0.01</v>
       </c>
@@ -767,7 +779,11 @@
       <c r="Q8" t="n">
         <v>6</v>
       </c>
-      <c r="R8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S8" t="n">
         <v>0.12</v>
       </c>
@@ -807,7 +823,11 @@
       <c r="Q9" t="n">
         <v>6</v>
       </c>
-      <c r="R9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S9" t="n">
         <v>0.01</v>
       </c>
@@ -847,7 +867,11 @@
       <c r="Q10" t="n">
         <v>24</v>
       </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S10" t="n">
         <v>0.00016875</v>
       </c>
@@ -887,7 +911,11 @@
       <c r="Q11" t="n">
         <v>6</v>
       </c>
-      <c r="R11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S11" t="n">
         <v>0.1</v>
       </c>
@@ -1121,7 +1149,11 @@
       <c r="Q16" t="n">
         <v>6</v>
       </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S16" t="n">
         <v>0.03</v>
       </c>
@@ -1161,7 +1193,11 @@
       <c r="Q17" t="n">
         <v>6</v>
       </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S17" t="n">
         <v>0.05</v>
       </c>
@@ -1201,7 +1237,11 @@
       <c r="Q18" t="n">
         <v>6</v>
       </c>
-      <c r="R18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S18" t="n">
         <v>0.05</v>
       </c>
@@ -1241,7 +1281,11 @@
       <c r="Q19" t="n">
         <v>24</v>
       </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S19" t="n">
         <v>0.00016875</v>
       </c>
@@ -1281,7 +1325,11 @@
       <c r="Q20" t="n">
         <v>6</v>
       </c>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S20" t="n">
         <v>0.09</v>
       </c>
@@ -1321,7 +1369,11 @@
       <c r="Q21" t="n">
         <v>6</v>
       </c>
-      <c r="R21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S21" t="n">
         <v>0.02</v>
       </c>
@@ -1361,7 +1413,11 @@
       <c r="Q22" t="n">
         <v>6</v>
       </c>
-      <c r="R22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S22" t="n">
         <v>0.02</v>
       </c>
@@ -1401,7 +1457,11 @@
       <c r="Q23" t="n">
         <v>6</v>
       </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S23" t="n">
         <v>0.01</v>
       </c>
@@ -1441,7 +1501,11 @@
       <c r="Q24" t="n">
         <v>6</v>
       </c>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S24" t="n">
         <v>0.004722000000000001</v>
       </c>
@@ -1675,7 +1739,11 @@
       <c r="Q29" t="n">
         <v>1</v>
       </c>
-      <c r="R29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S29" t="n">
         <v>0.12</v>
       </c>
@@ -1715,7 +1783,11 @@
       <c r="Q30" t="n">
         <v>1</v>
       </c>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S30" t="n">
         <v>0.12</v>
       </c>
@@ -1755,7 +1827,11 @@
       <c r="Q31" t="n">
         <v>1</v>
       </c>
-      <c r="R31" t="inlineStr"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S31" t="n">
         <v>0.01</v>
       </c>
@@ -1795,7 +1871,11 @@
       <c r="Q32" t="n">
         <v>1</v>
       </c>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S32" t="n">
         <v>0.01</v>
       </c>
@@ -1835,7 +1915,11 @@
       <c r="Q33" t="n">
         <v>1</v>
       </c>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S33" t="n">
         <v>0.03</v>
       </c>
@@ -1875,7 +1959,11 @@
       <c r="Q34" t="n">
         <v>1</v>
       </c>
-      <c r="R34" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S34" t="n">
         <v>0.00273735</v>
       </c>
@@ -1915,7 +2003,11 @@
       <c r="Q35" t="n">
         <v>1</v>
       </c>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S35" t="n">
         <v>0.03</v>
       </c>
@@ -1955,7 +2047,11 @@
       <c r="Q36" t="n">
         <v>1</v>
       </c>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S36" t="n">
         <v>0.00129402</v>
       </c>
@@ -1995,7 +2091,11 @@
       <c r="Q37" t="n">
         <v>1</v>
       </c>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S37" t="n">
         <v>0.1</v>
       </c>
@@ -2035,7 +2135,11 @@
       <c r="Q38" t="n">
         <v>1</v>
       </c>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S38" t="n">
         <v>0.03</v>
       </c>
@@ -2075,7 +2179,11 @@
       <c r="Q39" t="n">
         <v>4</v>
       </c>
-      <c r="R39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S39" t="n">
         <v>0.00016875</v>
       </c>
@@ -2309,7 +2417,11 @@
       <c r="Q44" t="n">
         <v>1</v>
       </c>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S44" t="n">
         <v>0.05</v>
       </c>
@@ -2349,7 +2461,11 @@
       <c r="Q45" t="n">
         <v>1</v>
       </c>
-      <c r="R45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S45" t="n">
         <v>0.05</v>
       </c>
@@ -2389,7 +2505,11 @@
       <c r="Q46" t="n">
         <v>1</v>
       </c>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S46" t="n">
         <v>0.03</v>
       </c>
@@ -2429,7 +2549,11 @@
       <c r="Q47" t="n">
         <v>1</v>
       </c>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S47" t="n">
         <v>0.03</v>
       </c>
@@ -2469,7 +2593,11 @@
       <c r="Q48" t="n">
         <v>1</v>
       </c>
-      <c r="R48" t="inlineStr"/>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S48" t="n">
         <v>0.09</v>
       </c>
@@ -2509,7 +2637,11 @@
       <c r="Q49" t="n">
         <v>2</v>
       </c>
-      <c r="R49" t="inlineStr"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S49" t="n">
         <v>0.02</v>
       </c>
@@ -2549,7 +2681,11 @@
       <c r="Q50" t="n">
         <v>4</v>
       </c>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S50" t="n">
         <v>0.00016875</v>
       </c>
@@ -2589,7 +2725,11 @@
       <c r="Q51" t="n">
         <v>1</v>
       </c>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S51" t="n">
         <v>0.02</v>
       </c>
@@ -2629,7 +2769,11 @@
       <c r="Q52" t="n">
         <v>1</v>
       </c>
-      <c r="R52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S52" t="n">
         <v>0.02</v>
       </c>
@@ -2669,7 +2813,11 @@
       <c r="Q53" t="n">
         <v>1</v>
       </c>
-      <c r="R53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S53" t="n">
         <v>0.0028332</v>
       </c>
@@ -2709,7 +2857,11 @@
       <c r="Q54" t="n">
         <v>1</v>
       </c>
-      <c r="R54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S54" t="n">
         <v>0.01</v>
       </c>
@@ -2943,7 +3095,11 @@
       <c r="Q59" t="n">
         <v>6</v>
       </c>
-      <c r="R59" t="inlineStr"/>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S59" t="n">
         <v>0.01</v>
       </c>
@@ -2983,7 +3139,11 @@
       <c r="Q60" t="n">
         <v>6</v>
       </c>
-      <c r="R60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S60" t="n">
         <v>0.01</v>
       </c>
@@ -3023,7 +3183,11 @@
       <c r="Q61" t="n">
         <v>6</v>
       </c>
-      <c r="R61" t="inlineStr"/>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S61" t="n">
         <v>0.01</v>
       </c>
@@ -3063,7 +3227,11 @@
       <c r="Q62" t="n">
         <v>6</v>
       </c>
-      <c r="R62" t="inlineStr"/>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S62" t="n">
         <v>0.01</v>
       </c>
@@ -3103,7 +3271,11 @@
       <c r="Q63" t="n">
         <v>6</v>
       </c>
-      <c r="R63" t="inlineStr"/>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S63" t="n">
         <v>0.02</v>
       </c>
@@ -3337,7 +3509,11 @@
       <c r="Q68" t="n">
         <v>6</v>
       </c>
-      <c r="R68" t="inlineStr"/>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S68" t="n">
         <v>0.01</v>
       </c>
@@ -3377,7 +3553,11 @@
       <c r="Q69" t="n">
         <v>6</v>
       </c>
-      <c r="R69" t="inlineStr"/>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S69" t="n">
         <v>0.07000000000000001</v>
       </c>
@@ -3417,7 +3597,11 @@
       <c r="Q70" t="n">
         <v>6</v>
       </c>
-      <c r="R70" t="inlineStr"/>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S70" t="n">
         <v>0.07000000000000001</v>
       </c>
@@ -3457,7 +3641,11 @@
       <c r="Q71" t="n">
         <v>6</v>
       </c>
-      <c r="R71" t="inlineStr"/>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S71" t="n">
         <v>0.05</v>
       </c>
@@ -3497,7 +3685,11 @@
       <c r="Q72" t="n">
         <v>24</v>
       </c>
-      <c r="R72" t="inlineStr"/>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S72" t="n">
         <v>0.00016875</v>
       </c>
@@ -3731,7 +3923,11 @@
       <c r="Q77" t="n">
         <v>6</v>
       </c>
-      <c r="R77" t="inlineStr"/>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S77" t="n">
         <v>0.01</v>
       </c>
@@ -3771,7 +3967,11 @@
       <c r="Q78" t="n">
         <v>6</v>
       </c>
-      <c r="R78" t="inlineStr"/>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S78" t="n">
         <v>0.01</v>
       </c>
@@ -3811,7 +4011,11 @@
       <c r="Q79" t="n">
         <v>6</v>
       </c>
-      <c r="R79" t="inlineStr"/>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S79" t="n">
         <v>0.02</v>
       </c>
@@ -3851,7 +4055,11 @@
       <c r="Q80" t="n">
         <v>6</v>
       </c>
-      <c r="R80" t="inlineStr"/>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S80" t="n">
         <v>0.02</v>
       </c>
@@ -3891,7 +4099,11 @@
       <c r="Q81" t="n">
         <v>6</v>
       </c>
-      <c r="R81" t="inlineStr"/>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S81" t="n">
         <v>0.03</v>
       </c>
@@ -4125,7 +4337,11 @@
       <c r="Q86" t="n">
         <v>2</v>
       </c>
-      <c r="R86" t="inlineStr"/>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S86" t="n">
         <v>0.01</v>
       </c>
@@ -4165,7 +4381,11 @@
       <c r="Q87" t="n">
         <v>2</v>
       </c>
-      <c r="R87" t="inlineStr"/>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S87" t="n">
         <v>0.01</v>
       </c>
@@ -4205,7 +4425,11 @@
       <c r="Q88" t="n">
         <v>2</v>
       </c>
-      <c r="R88" t="inlineStr"/>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S88" t="n">
         <v>0.01</v>
       </c>
@@ -4245,7 +4469,11 @@
       <c r="Q89" t="n">
         <v>2</v>
       </c>
-      <c r="R89" t="inlineStr"/>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S89" t="n">
         <v>0.004644</v>
       </c>
@@ -4285,7 +4513,11 @@
       <c r="Q90" t="n">
         <v>2</v>
       </c>
-      <c r="R90" t="inlineStr"/>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S90" t="n">
         <v>0.01</v>
       </c>
@@ -4519,7 +4751,11 @@
       <c r="Q95" t="n">
         <v>2</v>
       </c>
-      <c r="R95" t="inlineStr"/>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S95" t="n">
         <v>0.03</v>
       </c>
@@ -4559,7 +4795,11 @@
       <c r="Q96" t="n">
         <v>2</v>
       </c>
-      <c r="R96" t="inlineStr"/>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S96" t="n">
         <v>0.03</v>
       </c>
@@ -4599,7 +4839,11 @@
       <c r="Q97" t="n">
         <v>4</v>
       </c>
-      <c r="R97" t="inlineStr"/>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S97" t="n">
         <v>0.0037152</v>
       </c>
@@ -4639,7 +4883,11 @@
       <c r="Q98" t="n">
         <v>2</v>
       </c>
-      <c r="R98" t="inlineStr"/>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S98" t="n">
         <v>0.04</v>
       </c>
@@ -4679,7 +4927,11 @@
       <c r="Q99" t="n">
         <v>8</v>
       </c>
-      <c r="R99" t="inlineStr"/>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S99" t="n">
         <v>0.00016875</v>
       </c>
@@ -4913,7 +5165,11 @@
       <c r="Q104" t="n">
         <v>2</v>
       </c>
-      <c r="R104" t="inlineStr"/>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S104" t="n">
         <v>0.0037152</v>
       </c>
@@ -4953,7 +5209,11 @@
       <c r="Q105" t="n">
         <v>2</v>
       </c>
-      <c r="R105" t="inlineStr"/>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S105" t="n">
         <v>0.01</v>
       </c>
@@ -4993,7 +5253,11 @@
       <c r="Q106" t="n">
         <v>2</v>
       </c>
-      <c r="R106" t="inlineStr"/>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S106" t="n">
         <v>0.01</v>
       </c>
@@ -5033,7 +5297,11 @@
       <c r="Q107" t="n">
         <v>2</v>
       </c>
-      <c r="R107" t="inlineStr"/>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S107" t="n">
         <v>0.01</v>
       </c>
@@ -5073,7 +5341,11 @@
       <c r="Q108" t="n">
         <v>2</v>
       </c>
-      <c r="R108" t="inlineStr"/>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S108" t="n">
         <v>0.01</v>
       </c>
@@ -5307,7 +5579,11 @@
       <c r="Q113" t="n">
         <v>2</v>
       </c>
-      <c r="R113" t="inlineStr"/>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S113" t="n">
         <v>0.01</v>
       </c>
@@ -5347,7 +5623,11 @@
       <c r="Q114" t="n">
         <v>2</v>
       </c>
-      <c r="R114" t="inlineStr"/>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S114" t="n">
         <v>0.01</v>
       </c>
@@ -5387,7 +5667,11 @@
       <c r="Q115" t="n">
         <v>2</v>
       </c>
-      <c r="R115" t="inlineStr"/>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S115" t="n">
         <v>0.01</v>
       </c>
@@ -5427,7 +5711,11 @@
       <c r="Q116" t="n">
         <v>2</v>
       </c>
-      <c r="R116" t="inlineStr"/>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S116" t="n">
         <v>0.004644</v>
       </c>
@@ -5467,7 +5755,11 @@
       <c r="Q117" t="n">
         <v>2</v>
       </c>
-      <c r="R117" t="inlineStr"/>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
       <c r="S117" t="n">
         <v>0.01</v>
       </c>

</xml_diff>